<commit_message>
Updated Database and procedures
</commit_message>
<xml_diff>
--- a/RatingUniversity/Files/12_citiruemost_publikaciy_pps_vuza.xlsx
+++ b/RatingUniversity/Files/12_citiruemost_publikaciy_pps_vuza.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repositories\Raiting — копия\RatingUniversity\Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="citiruemost_publikaciy_pps_vuza" sheetId="1" r:id="rId1"/>
+    <sheet name="eng_lang" sheetId="1" r:id="rId1"/>
+    <sheet name="rus_uzb_lang" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="filename">citiruemost_publikaciy_pps_vuza!#REF!</definedName>
-    <definedName name="fio">citiruemost_publikaciy_pps_vuza!$B$7</definedName>
-    <definedName name="id">citiruemost_publikaciy_pps_vuza!$A$7</definedName>
-    <definedName name="info">citiruemost_publikaciy_pps_vuza!$D$7</definedName>
-    <definedName name="link">citiruemost_publikaciy_pps_vuza!$E$7</definedName>
-    <definedName name="name">citiruemost_publikaciy_pps_vuza!$B$7</definedName>
-    <definedName name="source">citiruemost_publikaciy_pps_vuza!$C$7</definedName>
-    <definedName name="usage">citiruemost_publikaciy_pps_vuza!$F$7</definedName>
+    <definedName name="filename">eng_lang!#REF!</definedName>
+    <definedName name="fio">eng_lang!$B$7</definedName>
+    <definedName name="id">eng_lang!$A$7</definedName>
+    <definedName name="info">eng_lang!$D$7</definedName>
+    <definedName name="link">eng_lang!$E$7</definedName>
+    <definedName name="name">eng_lang!$B$7</definedName>
+    <definedName name="source">eng_lang!$C$7</definedName>
+    <definedName name="usage">eng_lang!$F$7</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Муаллиф (лар) Ф.И.Ш.</t>
   </si>
@@ -44,23 +50,6 @@
   </si>
   <si>
     <t>...</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Чоп этилган материаллар номи </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>ва тили</t>
-    </r>
   </si>
   <si>
     <t>(муаллиф ОТМда фаолият олиб борган барча йиллар бўйича)</t>
@@ -149,12 +138,18 @@
       <t xml:space="preserve"> устунда келтирилмаган маълумотлар хисобга олинмайди.)</t>
     </r>
   </si>
+  <si>
+    <t>Чоп этилган материаллар номи (инглиз тилида)</t>
+  </si>
+  <si>
+    <t>Чоп этилган материаллар номи (рус ва узбек тилида)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,15 +169,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
@@ -296,7 +282,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -309,7 +295,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -596,7 +582,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -606,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -623,7 +609,7 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -633,7 +619,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -643,7 +629,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -653,7 +639,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -664,7 +650,7 @@
     <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:6" ht="121.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -673,7 +659,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>2</v>
@@ -732,7 +718,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -745,4 +731,167 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>4</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>